<commit_message>
Continuing the development of the Monty JSON Schema
</commit_message>
<xml_diff>
--- a/Taxonomies/MostlyImpactData/IFRC_HIP.xlsx
+++ b/Taxonomies/MostlyImpactData/IFRC_HIP.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="61">
   <si>
     <t xml:space="preserve">dtype</t>
   </si>
@@ -145,6 +145,9 @@
     <t xml:space="preserve">Civil Unrest</t>
   </si>
   <si>
+    <t xml:space="preserve">haztypesoc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Drought</t>
   </si>
   <si>
@@ -178,6 +181,9 @@
     <t xml:space="preserve">Transport Accident</t>
   </si>
   <si>
+    <t xml:space="preserve">haztypetech</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tsunami</t>
   </si>
   <si>
@@ -188,6 +194,9 @@
   </si>
   <si>
     <t xml:space="preserve">Chemical Emergency</t>
+  </si>
+  <si>
+    <t xml:space="preserve">haztypechem</t>
   </si>
   <si>
     <t xml:space="preserve">Insect Infestation</t>
@@ -298,7 +307,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -470,90 +479,105 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
+      <c r="C14" s="0" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>57</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>59</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>57</v>
+        <v>60</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>